<commit_message>
better movies than finki's movies
</commit_message>
<xml_diff>
--- a/Integrirani Sistemi/Lab5/Movies.xlsx
+++ b/Integrirani Sistemi/Lab5/Movies.xlsx
@@ -1,77 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27718"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefani K\Downloads\Lab4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B686BDAD-E523-4EAA-AC51-67526F7D0828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B80A04F8-FFCB-42E0-85E6-1E0CD20EC43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Movie1</t>
-  </si>
-  <si>
-    <t>Movie1 desc</t>
-  </si>
-  <si>
-    <t>Movie2</t>
-  </si>
-  <si>
-    <t>Movie2 desc</t>
-  </si>
-  <si>
-    <t>Movie3</t>
-  </si>
-  <si>
-    <t>Movie3 desc</t>
-  </si>
-  <si>
-    <t>Movie4</t>
-  </si>
-  <si>
-    <t>Movie4 desc</t>
-  </si>
-  <si>
-    <t>https://img.freepik.com/free-photo/composition-cinema-elements-pink-background-with-copy-space_23-2148416788.jpg?w=996&amp;t=st=1716137523~exp=1716138123~hmac=a60dd54121ed37bc14af85f56aae2556b340bcf76344e68a31b537f21ff75c3b</t>
-  </si>
-  <si>
-    <t>https://img.freepik.com/free-photo/clapperboard-popcorn-film-stripe-cinema-tickets-wooden-desk_23-2148188189.jpg?w=996&amp;t=st=1716137548~exp=1716138148~hmac=ad6ea89743e922b926296686728ba30bfc457152f615e31fa939d977cb84be54</t>
-  </si>
-  <si>
-    <t>https://img.freepik.com/free-photo/rows-red-seats-theater_53876-64710.jpg?w=1060&amp;t=st=1716137613~exp=1716138213~hmac=08b633e81811867ce5645084893c17da5c55c0fe3ca2e958240c6a1a1cf2c92a</t>
-  </si>
-  <si>
-    <t>https://img.freepik.com/free-psd/3d-cinema-blank-banner-background_23-2150822408.jpg?w=996&amp;t=st=1716137639~exp=1716138239~hmac=e96a9a19c315d671ad36efac426e2769f507a0c83371f77e694037967205215f</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>The Dark Knight Rises</t>
+  </si>
+  <si>
+    <t>A movie about a nigga dick that gets a boner</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/M/MV5BODZkYTdhMzQtYzMxYi00OGVjLTgzOTEtYTU5OTBjZDljZDM5XkEyXkFqcGdeQXVyNjczMzc5NzQ@._V1_FMjpg_UX1000_.jpg</t>
+  </si>
+  <si>
+    <t>Anyone But You</t>
+  </si>
+  <si>
+    <t>A funny movie</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/S/pv-target-images/ef4bf79819e44f6f2e46f2acb0079b431fa3627def069ab4304c03384a87df7d.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -79,7 +67,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -114,7 +102,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -137,39 +125,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -202,9 +190,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -237,6 +242,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -298,13 +320,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -313,6 +328,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -377,7 +399,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -389,19 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,60 +447,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
+        <v>100000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{14188A74-5A69-42A5-A82B-9E31514B0ACD}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{616BD991-11D2-4DDC-836C-47EDDAF8598F}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{5E823F8F-2F01-4F05-9A92-D3B9F95D1F05}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{D90798A7-BB8D-4160-B48B-A4CAAE56C9C9}"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{BFCAC32E-CC21-425B-BAB1-8DECB71A03D0}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{1C7FF835-C43A-41E4-B213-5F95774256FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>